<commit_message>
Har opdateret den måde jeg eksporterer resultater fra alle modeller og jeg har oprettet første statistiske test
</commit_message>
<xml_diff>
--- a/Fase3_ValueBettingAnalysis/NeuralNetworkOutliers/PercentagePointDifference/30pointDifferenceOutliers.xlsx
+++ b/Fase3_ValueBettingAnalysis/NeuralNetworkOutliers/PercentagePointDifference/30pointDifferenceOutliers.xlsx
@@ -681,13 +681,13 @@
         <v>0.2</v>
       </c>
       <c r="W2" t="n">
-        <v>0.6509307622909546</v>
+        <v>0.6608967185020447</v>
       </c>
       <c r="X2" t="n">
-        <v>0.2135529071092606</v>
+        <v>0.2107896357774734</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.1355163156986237</v>
+        <v>0.1283136308193207</v>
       </c>
       <c r="Z2" t="n">
         <v>0.3143562518529746</v>
@@ -699,22 +699,22 @@
         <v>0.2602437356586661</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.33657451043798</v>
+        <v>0.3465404666490701</v>
       </c>
       <c r="AD2" t="n">
-        <v>-0.2118471053790987</v>
+        <v>-0.2146103767108858</v>
       </c>
       <c r="AE2" t="n">
-        <v>-0.1247274199600424</v>
+        <v>-0.1319301048393454</v>
       </c>
       <c r="AF2" t="n">
-        <v>107.0678596191549</v>
+        <v>110.2381341571499</v>
       </c>
       <c r="AG2" t="n">
-        <v>-49.79950614949635</v>
+        <v>-50.44907626013727</v>
       </c>
       <c r="AH2" t="n">
-        <v>-47.92715553531481</v>
+        <v>-50.69482441351981</v>
       </c>
     </row>
     <row r="3">
@@ -793,13 +793,13 @@
         <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>0.6446380615234375</v>
+        <v>0.6515154242515564</v>
       </c>
       <c r="X3" t="n">
-        <v>0.220141589641571</v>
+        <v>0.2179467082023621</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.1352203637361526</v>
+        <v>0.1305378526449203</v>
       </c>
       <c r="Z3" t="n">
         <v>0.2962041139150656</v>
@@ -811,22 +811,22 @@
         <v>0.281794533329756</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.3484339476083719</v>
+        <v>0.3553113103364908</v>
       </c>
       <c r="AD3" t="n">
-        <v>-0.2018597631136074</v>
+        <v>-0.2040546445528164</v>
       </c>
       <c r="AE3" t="n">
-        <v>-0.1465741695936034</v>
+        <v>-0.1512566806848357</v>
       </c>
       <c r="AF3" t="n">
-        <v>117.6330547887943</v>
+        <v>119.9548870676299</v>
       </c>
       <c r="AG3" t="n">
-        <v>-47.83391375304787</v>
+        <v>-48.354026170906</v>
       </c>
       <c r="AH3" t="n">
-        <v>-52.01455395945607</v>
+        <v>-53.67622959095344</v>
       </c>
     </row>
     <row r="4">
@@ -905,13 +905,13 @@
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>0.5987902879714966</v>
+        <v>0.5967223644256592</v>
       </c>
       <c r="X4" t="n">
-        <v>0.2358331680297852</v>
+        <v>0.2387918680906296</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.1653765439987183</v>
+        <v>0.1644857674837112</v>
       </c>
       <c r="Z4" t="n">
         <v>0.2729387142374602</v>
@@ -923,28 +923,28 @@
         <v>0.2767748170377056</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.3258515737340364</v>
+        <v>0.323783650188199</v>
       </c>
       <c r="AD4" t="n">
-        <v>-0.214453300695049</v>
+        <v>-0.2114946006342046</v>
       </c>
       <c r="AE4" t="n">
-        <v>-0.1113982730389874</v>
+        <v>-0.1122890495539944</v>
       </c>
       <c r="AF4" t="n">
-        <v>119.3863518571943</v>
+        <v>118.6287006197674</v>
       </c>
       <c r="AG4" t="n">
-        <v>-47.62597048549097</v>
+        <v>-46.96889987237146</v>
       </c>
       <c r="AH4" t="n">
-        <v>-40.24870262087874</v>
+        <v>-40.57054422646299</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>27/02/2019</t>
+          <t>04/11/2018</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -954,7 +954,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>West Ham</t>
+          <t>Southampton</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -963,25 +963,25 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4.61038961038961</v>
+        <v>4.675324675324675</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="G5" t="n">
-        <v>2.4</v>
+        <v>2.6</v>
       </c>
       <c r="H5" t="n">
-        <v>14.6</v>
+        <v>18.4</v>
       </c>
       <c r="I5" t="n">
-        <v>6.6</v>
+        <v>7.2</v>
       </c>
       <c r="J5" t="n">
         <v>8.4</v>
       </c>
       <c r="K5" t="n">
-        <v>4.8</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="L5" t="n">
         <v>1.6</v>
@@ -990,195 +990,195 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>1.363636363636364</v>
+        <v>1.428571428571428</v>
       </c>
       <c r="O5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="Q5" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="R5" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="S5" t="n">
         <v>10.6</v>
       </c>
-      <c r="R5" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="S5" t="n">
-        <v>9.800000000000001</v>
-      </c>
       <c r="T5" t="n">
-        <v>4.4</v>
+        <v>5</v>
       </c>
       <c r="U5" t="n">
-        <v>0.8</v>
+        <v>2.2</v>
       </c>
       <c r="V5" t="n">
         <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>0.7772766947746277</v>
+        <v>0.806554913520813</v>
       </c>
       <c r="X5" t="n">
-        <v>0.1553220003843307</v>
+        <v>0.1382298618555069</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.06740126013755798</v>
+        <v>0.05521528422832489</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.4524206900186175</v>
+        <v>0.5050918173100506</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.3752872575035762</v>
+        <v>0.3524422046309223</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.1722920524778064</v>
+        <v>0.1424659780590271</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.3248560047560102</v>
+        <v>0.3014630962107624</v>
       </c>
       <c r="AD5" t="n">
-        <v>-0.2199652571192455</v>
+        <v>-0.2142123427754154</v>
       </c>
       <c r="AE5" t="n">
-        <v>-0.1048907923402484</v>
+        <v>-0.08725069383070222</v>
       </c>
       <c r="AF5" t="n">
-        <v>71.8039673965048</v>
+        <v>59.68481093521839</v>
       </c>
       <c r="AG5" t="n">
-        <v>-58.6125035479387</v>
+        <v>-60.77942424623598</v>
       </c>
       <c r="AH5" t="n">
-        <v>-60.87964640955206</v>
+        <v>-61.24317891149572</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>21/04/2019</t>
+          <t>27/02/2019</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Arsenal</t>
+          <t>Man City</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Crystal Palace</t>
+          <t>West Ham</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>H</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>3.636363636363637</v>
+        <v>4.61038961038961</v>
       </c>
       <c r="F6" t="n">
-        <v>1.2</v>
+        <v>3</v>
       </c>
       <c r="G6" t="n">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="H6" t="n">
-        <v>11.2</v>
+        <v>14.6</v>
       </c>
       <c r="I6" t="n">
-        <v>3.8</v>
+        <v>6.6</v>
       </c>
       <c r="J6" t="n">
-        <v>10.8</v>
+        <v>8.4</v>
       </c>
       <c r="K6" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="L6" t="n">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="M6" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>2.207792207792208</v>
+        <v>1.363636363636364</v>
       </c>
       <c r="O6" t="n">
         <v>1</v>
       </c>
       <c r="P6" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="Q6" t="n">
+        <v>10.6</v>
+      </c>
+      <c r="R6" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="S6" t="n">
         <v>9.800000000000001</v>
       </c>
-      <c r="R6" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="S6" t="n">
-        <v>8.199999999999999</v>
-      </c>
       <c r="T6" t="n">
-        <v>4.2</v>
+        <v>4.4</v>
       </c>
       <c r="U6" t="n">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="V6" t="n">
         <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>0.6194396018981934</v>
+        <v>0.7797143459320068</v>
       </c>
       <c r="X6" t="n">
-        <v>0.2309439331293106</v>
+        <v>0.1545599550008774</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.1496164947748184</v>
+        <v>0.0657256618142128</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.2830072236890522</v>
+        <v>0.4524206900186175</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.4206162407121692</v>
+        <v>0.3752872575035762</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.2963765355987786</v>
+        <v>0.1722920524778064</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.3364323782091412</v>
+        <v>0.3272936559133893</v>
       </c>
       <c r="AD6" t="n">
-        <v>-0.1896723075828586</v>
+        <v>-0.2207273025026988</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0.1467600408239602</v>
+        <v>-0.1065663906635936</v>
       </c>
       <c r="AF6" t="n">
-        <v>118.8776646135325</v>
+        <v>72.34276927076895</v>
       </c>
       <c r="AG6" t="n">
-        <v>-45.09390965544118</v>
+        <v>-58.8155601048073</v>
       </c>
       <c r="AH6" t="n">
-        <v>-49.51810389694189</v>
+        <v>-61.85218013890735</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16/09/2018</t>
+          <t>21/04/2019</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Everton</t>
+          <t>Arsenal</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>West Ham</t>
+          <t>Crystal Palace</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1187,100 +1187,100 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>2.337662337662338</v>
+        <v>3.636363636363637</v>
       </c>
       <c r="F7" t="n">
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
       <c r="G7" t="n">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="H7" t="n">
-        <v>11</v>
+        <v>11.2</v>
       </c>
       <c r="I7" t="n">
-        <v>4.6</v>
+        <v>3.8</v>
       </c>
       <c r="J7" t="n">
-        <v>10.2</v>
+        <v>10.8</v>
       </c>
       <c r="K7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L7" t="n">
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="M7" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="N7" t="n">
-        <v>1.493506493506493</v>
+        <v>2.207792207792208</v>
       </c>
       <c r="O7" t="n">
         <v>1</v>
       </c>
       <c r="P7" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="R7" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="S7" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="T7" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="U7" t="n">
         <v>0.6</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>11.4</v>
-      </c>
-      <c r="R7" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="S7" t="n">
-        <v>11.2</v>
-      </c>
-      <c r="T7" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="U7" t="n">
-        <v>2.6</v>
       </c>
       <c r="V7" t="n">
         <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>0.496292382478714</v>
+        <v>0.6233481764793396</v>
       </c>
       <c r="X7" t="n">
-        <v>0.2736426293849945</v>
+        <v>0.2296731024980545</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.2300649583339691</v>
+        <v>0.1469787061214447</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.1901203196054265</v>
+        <v>0.2830072236890522</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.4068781578506765</v>
+        <v>0.4206162407121692</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.403001522543897</v>
+        <v>0.2963765355987786</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.3061720628732875</v>
+        <v>0.3403409527902874</v>
       </c>
       <c r="AD7" t="n">
-        <v>-0.133235528465682</v>
+        <v>-0.1909431382141147</v>
       </c>
       <c r="AE7" t="n">
-        <v>-0.1729365642099279</v>
+        <v>-0.1493978294773339</v>
       </c>
       <c r="AF7" t="n">
-        <v>161.0412098552713</v>
+        <v>120.2587511208652</v>
       </c>
       <c r="AG7" t="n">
-        <v>-32.74580507577385</v>
+        <v>-45.39604507206332</v>
       </c>
       <c r="AH7" t="n">
-        <v>-42.91213668829024</v>
+        <v>-50.40811654522545</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>21/10/2018</t>
+          <t>16/09/2018</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1290,119 +1290,119 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Crystal Palace</t>
+          <t>West Ham</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E8" t="n">
         <v>2.337662337662338</v>
       </c>
       <c r="F8" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="G8" t="n">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="H8" t="n">
-        <v>14.4</v>
+        <v>11</v>
       </c>
       <c r="I8" t="n">
-        <v>5</v>
+        <v>4.6</v>
       </c>
       <c r="J8" t="n">
-        <v>12.8</v>
+        <v>10.2</v>
       </c>
       <c r="K8" t="n">
-        <v>7.8</v>
+        <v>4</v>
       </c>
       <c r="L8" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="N8" t="n">
-        <v>2.272727272727272</v>
+        <v>1.493506493506493</v>
       </c>
       <c r="O8" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="P8" t="n">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="Q8" t="n">
-        <v>12.8</v>
+        <v>11.4</v>
       </c>
       <c r="R8" t="n">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="S8" t="n">
-        <v>11.8</v>
+        <v>11.2</v>
       </c>
       <c r="T8" t="n">
-        <v>5.6</v>
+        <v>4.4</v>
       </c>
       <c r="U8" t="n">
-        <v>2.2</v>
+        <v>2.6</v>
       </c>
       <c r="V8" t="n">
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>0.5201937556266785</v>
+        <v>0.5013116002082825</v>
       </c>
       <c r="X8" t="n">
-        <v>0.2618935704231262</v>
+        <v>0.2708079218864441</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.2179126143455505</v>
+        <v>0.2278804928064346</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.209133710096302</v>
+        <v>0.1901203196054265</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.4401212211619819</v>
+        <v>0.4068781578506765</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.3507450687417161</v>
+        <v>0.403001522543897</v>
       </c>
       <c r="AC8" t="n">
-        <v>0.3110600455303765</v>
+        <v>0.3111912806028559</v>
       </c>
       <c r="AD8" t="n">
-        <v>-0.1782276507388557</v>
+        <v>-0.1360702359642324</v>
       </c>
       <c r="AE8" t="n">
-        <v>-0.1328324543961656</v>
+        <v>-0.1751210297374624</v>
       </c>
       <c r="AF8" t="n">
-        <v>148.7374012478139</v>
+        <v>163.6812315741414</v>
       </c>
       <c r="AG8" t="n">
-        <v>-40.49512774419502</v>
+        <v>-33.44250197233982</v>
       </c>
       <c r="AH8" t="n">
-        <v>-37.87151017481064</v>
+        <v>-43.45418563980419</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>22/09/2018</t>
+          <t>21/10/2018</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Everton</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Southampton</t>
+          <t>Crystal Palace</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1411,110 +1411,110 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>3.831168831168831</v>
+        <v>2.337662337662338</v>
       </c>
       <c r="F9" t="n">
-        <v>2.2</v>
+        <v>1.4</v>
       </c>
       <c r="G9" t="n">
-        <v>3</v>
+        <v>1.4</v>
       </c>
       <c r="H9" t="n">
-        <v>16.6</v>
+        <v>14.4</v>
       </c>
       <c r="I9" t="n">
-        <v>7.2</v>
+        <v>5</v>
       </c>
       <c r="J9" t="n">
-        <v>12.6</v>
+        <v>12.8</v>
       </c>
       <c r="K9" t="n">
-        <v>5.6</v>
+        <v>7.8</v>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>1.428571428571428</v>
+        <v>2.272727272727272</v>
       </c>
       <c r="O9" t="n">
-        <v>1.2</v>
+        <v>0.4</v>
       </c>
       <c r="P9" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="Q9" t="n">
-        <v>15.4</v>
+        <v>12.8</v>
       </c>
       <c r="R9" t="n">
-        <v>4.6</v>
+        <v>3.6</v>
       </c>
       <c r="S9" t="n">
-        <v>13</v>
+        <v>11.8</v>
       </c>
       <c r="T9" t="n">
         <v>5.6</v>
       </c>
       <c r="U9" t="n">
-        <v>1.8</v>
+        <v>2.2</v>
       </c>
       <c r="V9" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>0.6915346384048462</v>
+        <v>0.5288232564926147</v>
       </c>
       <c r="X9" t="n">
-        <v>0.1967647969722748</v>
+        <v>0.2610736191272736</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.1117005422711372</v>
+        <v>0.2101031541824341</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.3909582976207729</v>
+        <v>0.209133710096302</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.4202645814934624</v>
+        <v>0.4401212211619819</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.1887771208857646</v>
+        <v>0.3507450687417161</v>
       </c>
       <c r="AC9" t="n">
-        <v>0.3005763407840733</v>
+        <v>0.3196895463963128</v>
       </c>
       <c r="AD9" t="n">
-        <v>-0.2234997845211876</v>
+        <v>-0.1790476020347083</v>
       </c>
       <c r="AE9" t="n">
-        <v>-0.07707657861462736</v>
+        <v>-0.140641914559282</v>
       </c>
       <c r="AF9" t="n">
-        <v>76.88194434374954</v>
+        <v>152.8637091787364</v>
       </c>
       <c r="AG9" t="n">
-        <v>-53.18073289139745</v>
+        <v>-40.68142898495044</v>
       </c>
       <c r="AH9" t="n">
-        <v>-40.82940679091562</v>
+        <v>-40.0980447319842</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>30/03/2019</t>
+          <t>22/09/2018</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Leicester</t>
+          <t>Liverpool</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bournemouth</t>
+          <t>Southampton</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1523,34 +1523,34 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2.37012987012987</v>
+        <v>3.831168831168831</v>
       </c>
       <c r="F10" t="n">
-        <v>1.8</v>
+        <v>2.2</v>
       </c>
       <c r="G10" t="n">
-        <v>1.8</v>
+        <v>3</v>
       </c>
       <c r="H10" t="n">
-        <v>17.4</v>
+        <v>16.6</v>
       </c>
       <c r="I10" t="n">
-        <v>4.4</v>
+        <v>7.2</v>
       </c>
       <c r="J10" t="n">
-        <v>8.800000000000001</v>
+        <v>12.6</v>
       </c>
       <c r="K10" t="n">
-        <v>5.2</v>
+        <v>5.6</v>
       </c>
       <c r="L10" t="n">
         <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>0.7467532467532467</v>
+        <v>1.428571428571428</v>
       </c>
       <c r="O10" t="n">
         <v>1.2</v>
@@ -1559,58 +1559,58 @@
         <v>1</v>
       </c>
       <c r="Q10" t="n">
-        <v>8.199999999999999</v>
+        <v>15.4</v>
       </c>
       <c r="R10" t="n">
-        <v>3.2</v>
+        <v>4.6</v>
       </c>
       <c r="S10" t="n">
-        <v>8.800000000000001</v>
+        <v>13</v>
       </c>
       <c r="T10" t="n">
-        <v>4.8</v>
+        <v>5.6</v>
       </c>
       <c r="U10" t="n">
-        <v>2.2</v>
+        <v>1.8</v>
       </c>
       <c r="V10" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="W10" t="n">
-        <v>0.5269556045532227</v>
+        <v>0.6941421627998352</v>
       </c>
       <c r="X10" t="n">
-        <v>0.260079026222229</v>
+        <v>0.1966769993305206</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.2129653692245483</v>
+        <v>0.1091808751225471</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.2249931865467219</v>
+        <v>0.3909582976207729</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.4156559935219178</v>
+        <v>0.4202645814934624</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.3593508199313602</v>
+        <v>0.1887771208857646</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.3019624180065008</v>
+        <v>0.3031838651790623</v>
       </c>
       <c r="AD10" t="n">
-        <v>-0.1555769672996888</v>
+        <v>-0.2235875821629418</v>
       </c>
       <c r="AE10" t="n">
-        <v>-0.1463854507068119</v>
+        <v>-0.07959624576321744</v>
       </c>
       <c r="AF10" t="n">
-        <v>134.2095832505557</v>
+        <v>77.54890151305824</v>
       </c>
       <c r="AG10" t="n">
-        <v>-37.42926114969761</v>
+        <v>-53.20162393138045</v>
       </c>
       <c r="AH10" t="n">
-        <v>-40.73608367855485</v>
+        <v>-42.16413800027378</v>
       </c>
     </row>
     <row r="11">
@@ -1689,13 +1689,13 @@
         <v>0.2</v>
       </c>
       <c r="W11" t="n">
-        <v>0.6872597932815552</v>
+        <v>0.7039117813110352</v>
       </c>
       <c r="X11" t="n">
-        <v>0.2024488598108292</v>
+        <v>0.195863738656044</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.1102913469076157</v>
+        <v>0.1002245545387268</v>
       </c>
       <c r="Z11" t="n">
         <v>0.3257455446787606</v>
@@ -1707,22 +1707,22 @@
         <v>0.2556153329567962</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.3615142486027946</v>
+        <v>0.3781662366322746</v>
       </c>
       <c r="AD11" t="n">
-        <v>-0.2161902625536141</v>
+        <v>-0.2227753837083993</v>
       </c>
       <c r="AE11" t="n">
-        <v>-0.1453239860491806</v>
+        <v>-0.1553907784180694</v>
       </c>
       <c r="AF11" t="n">
-        <v>110.9805658153538</v>
+        <v>116.0925276829832</v>
       </c>
       <c r="AG11" t="n">
-        <v>-51.64119906725087</v>
+        <v>-53.21418181133672</v>
       </c>
       <c r="AH11" t="n">
-        <v>-56.85260910140435</v>
+        <v>-60.79086751980304</v>
       </c>
     </row>
     <row r="12">
@@ -1801,13 +1801,13 @@
         <v>0.4</v>
       </c>
       <c r="W12" t="n">
-        <v>0.611750602722168</v>
+        <v>0.608129620552063</v>
       </c>
       <c r="X12" t="n">
-        <v>0.2305290997028351</v>
+        <v>0.2323235273361206</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.1577203422784805</v>
+        <v>0.159546822309494</v>
       </c>
       <c r="Z12" t="n">
         <v>0.269763972484084</v>
@@ -1819,22 +1819,22 @@
         <v>0.3044242467002724</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.341986630238084</v>
+        <v>0.338365648067979</v>
       </c>
       <c r="AD12" t="n">
-        <v>-0.1952826811128085</v>
+        <v>-0.193488253479523</v>
       </c>
       <c r="AE12" t="n">
-        <v>-0.1467039044217919</v>
+        <v>-0.1448774243907784</v>
       </c>
       <c r="AF12" t="n">
-        <v>126.7725364098651</v>
+        <v>125.4302585153184</v>
       </c>
       <c r="AG12" t="n">
-        <v>-45.86126779741603</v>
+        <v>-45.43985446078916</v>
       </c>
       <c r="AH12" t="n">
-        <v>-48.19061096872235</v>
+        <v>-47.5906324680572</v>
       </c>
     </row>
     <row r="13">
@@ -1913,13 +1913,13 @@
         <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>0.6067691445350647</v>
+        <v>0.6095803380012512</v>
       </c>
       <c r="X13" t="n">
-        <v>0.2303281724452972</v>
+        <v>0.2303340882062912</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.1629026681184769</v>
+        <v>0.1600855737924576</v>
       </c>
       <c r="Z13" t="n">
         <v>0.2594807254327272</v>
@@ -1931,28 +1931,28 @@
         <v>0.3127240778206081</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.3472884191023375</v>
+        <v>0.350099612568524</v>
       </c>
       <c r="AD13" t="n">
-        <v>-0.1974670243013675</v>
+        <v>-0.1974611085403735</v>
       </c>
       <c r="AE13" t="n">
-        <v>-0.1498214097021313</v>
+        <v>-0.1526385040281505</v>
       </c>
       <c r="AF13" t="n">
-        <v>133.8397750057066</v>
+        <v>134.9231670231671</v>
       </c>
       <c r="AG13" t="n">
-        <v>-46.15924297492875</v>
+        <v>-46.15786012607048</v>
       </c>
       <c r="AH13" t="n">
-        <v>-47.90849836259657</v>
+        <v>-48.80932261177232</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>15/12/2018</t>
+          <t>14/01/2019</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1962,7 +1962,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Everton</t>
+          <t>Wolves</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -1971,105 +1971,105 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>4.675324675324675</v>
+        <v>4.61038961038961</v>
       </c>
       <c r="F14" t="n">
-        <v>2.4</v>
+        <v>2.2</v>
       </c>
       <c r="G14" t="n">
-        <v>2.4</v>
+        <v>1.8</v>
       </c>
       <c r="H14" t="n">
-        <v>14.2</v>
+        <v>13.2</v>
       </c>
       <c r="I14" t="n">
-        <v>5.6</v>
+        <v>4.8</v>
       </c>
       <c r="J14" t="n">
-        <v>8.6</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="K14" t="n">
-        <v>7.6</v>
+        <v>7.2</v>
       </c>
       <c r="L14" t="n">
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="N14" t="n">
-        <v>2.337662337662338</v>
+        <v>1.883116883116883</v>
       </c>
       <c r="O14" t="n">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="P14" t="n">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="Q14" t="n">
-        <v>12.4</v>
+        <v>10.8</v>
       </c>
       <c r="R14" t="n">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="S14" t="n">
-        <v>10</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="T14" t="n">
-        <v>6.6</v>
+        <v>3.2</v>
       </c>
       <c r="U14" t="n">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="V14" t="n">
         <v>0</v>
       </c>
       <c r="W14" t="n">
-        <v>0.718335747718811</v>
+        <v>0.7305483222007751</v>
       </c>
       <c r="X14" t="n">
-        <v>0.1851275116205215</v>
+        <v>0.1797405630350113</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.09653674066066742</v>
+        <v>0.08971118927001953</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.3933788567781544</v>
+        <v>0.4167950619905854</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.3936515946035148</v>
+        <v>0.3936744963329367</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.2129695486183307</v>
+        <v>0.1895304416764778</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.3249568909406567</v>
+        <v>0.3137532602101897</v>
       </c>
       <c r="AD14" t="n">
-        <v>-0.2085240829829932</v>
+        <v>-0.2139339332979254</v>
       </c>
       <c r="AE14" t="n">
-        <v>-0.1164328079576633</v>
+        <v>-0.09981925240645828</v>
       </c>
       <c r="AF14" t="n">
-        <v>82.60659802667428</v>
+        <v>75.27758575442931</v>
       </c>
       <c r="AG14" t="n">
-        <v>-52.97173588056167</v>
+        <v>-54.34284803580422</v>
       </c>
       <c r="AH14" t="n">
-        <v>-54.6711061337347</v>
+        <v>-52.66660675905902</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>28/10/2018</t>
+          <t>15/12/2018</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Man United</t>
+          <t>Man City</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -2083,52 +2083,52 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>3.181818181818182</v>
+        <v>4.675324675324675</v>
       </c>
       <c r="F15" t="n">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="G15" t="n">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="H15" t="n">
-        <v>11.6</v>
+        <v>14.2</v>
       </c>
       <c r="I15" t="n">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="J15" t="n">
-        <v>12.2</v>
+        <v>8.6</v>
       </c>
       <c r="K15" t="n">
-        <v>7</v>
+        <v>7.6</v>
       </c>
       <c r="L15" t="n">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="M15" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="N15" t="n">
         <v>2.337662337662338</v>
       </c>
       <c r="O15" t="n">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="P15" t="n">
-        <v>1.8</v>
+        <v>1.2</v>
       </c>
       <c r="Q15" t="n">
-        <v>16.2</v>
+        <v>12.4</v>
       </c>
       <c r="R15" t="n">
-        <v>5.6</v>
+        <v>4</v>
       </c>
       <c r="S15" t="n">
-        <v>12.8</v>
+        <v>10</v>
       </c>
       <c r="T15" t="n">
-        <v>9</v>
+        <v>6.6</v>
       </c>
       <c r="U15" t="n">
         <v>1.2</v>
@@ -2137,40 +2137,40 @@
         <v>0</v>
       </c>
       <c r="W15" t="n">
-        <v>0.5295895934104919</v>
+        <v>0.7295903563499451</v>
       </c>
       <c r="X15" t="n">
-        <v>0.2602070271968842</v>
+        <v>0.1797457933425903</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.2102033346891403</v>
+        <v>0.09066393971443176</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.2249042356385522</v>
+        <v>0.3933788567781544</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.4374948738347362</v>
+        <v>0.3936515946035148</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.3376008905267116</v>
+        <v>0.2129695486183307</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.3046853577719397</v>
+        <v>0.3362114995717907</v>
       </c>
       <c r="AD15" t="n">
-        <v>-0.177287846637852</v>
+        <v>-0.2139058012609245</v>
       </c>
       <c r="AE15" t="n">
-        <v>-0.1273975558375713</v>
+        <v>-0.1223056089038989</v>
       </c>
       <c r="AF15" t="n">
-        <v>135.4733746596063</v>
+        <v>85.46760807772566</v>
       </c>
       <c r="AG15" t="n">
-        <v>-40.52341118511541</v>
+        <v>-54.33886314530747</v>
       </c>
       <c r="AH15" t="n">
-        <v>-37.73614330187656</v>
+        <v>-57.4286839115608</v>
       </c>
     </row>
     <row r="16">
@@ -2249,13 +2249,13 @@
         <v>0.2</v>
       </c>
       <c r="W16" t="n">
-        <v>0.6647847890853882</v>
+        <v>0.6637383103370667</v>
       </c>
       <c r="X16" t="n">
-        <v>0.2131295055150986</v>
+        <v>0.21444071829319</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.1220857203006744</v>
+        <v>0.1218210458755493</v>
       </c>
       <c r="Z16" t="n">
         <v>0.3432523593195986</v>
@@ -2267,22 +2267,22 @@
         <v>0.2233791720408737</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.3215324297657896</v>
+        <v>0.3204859510174681</v>
       </c>
       <c r="AD16" t="n">
-        <v>-0.2202389631244293</v>
+        <v>-0.2189277503463378</v>
       </c>
       <c r="AE16" t="n">
-        <v>-0.1012934517401993</v>
+        <v>-0.1015581261653244</v>
       </c>
       <c r="AF16" t="n">
-        <v>93.67231456271338</v>
+        <v>93.36744302435139</v>
       </c>
       <c r="AG16" t="n">
-        <v>-50.82025552431737</v>
+        <v>-50.51769249239959</v>
       </c>
       <c r="AH16" t="n">
-        <v>-45.34596973153106</v>
+        <v>-45.46445634901958</v>
       </c>
     </row>
   </sheetData>

</xml_diff>